<commit_message>
add ucrr(d) and test cases
</commit_message>
<xml_diff>
--- a/docs/W-9 Working Document/W-9.2 Requirements/vms_gap_analysis_v0.1.xlsx
+++ b/docs/W-9 Working Document/W-9.2 Requirements/vms_gap_analysis_v0.1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Gap Analysis" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Gap Analysis'!$A$1:$G$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Gap Analysis'!$A$1:$F$41</definedName>
     <definedName name="_Toc300993748" localSheetId="0">'Gap Analysis'!$C$20</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
   <si>
     <t>No</t>
   </si>
@@ -32,9 +32,6 @@
     <t>URS Clause No.</t>
   </si>
   <si>
-    <t>UCMS Use Case</t>
-  </si>
-  <si>
     <t>UCRR (Analysis)</t>
   </si>
   <si>
@@ -294,6 +291,123 @@
   </si>
   <si>
     <t>Source Code</t>
+  </si>
+  <si>
+    <t>1.2.1.1 Login</t>
+  </si>
+  <si>
+    <t>1.2.1.3 Logout</t>
+  </si>
+  <si>
+    <t>1.2.1.2 Change Password</t>
+  </si>
+  <si>
+    <t>1.2.1.4 Forget Password</t>
+  </si>
+  <si>
+    <t>3. Update Profile</t>
+  </si>
+  <si>
+    <t>2. Register Volunteer Account</t>
+  </si>
+  <si>
+    <t>4. Browse Projects</t>
+  </si>
+  <si>
+    <t>5. Raise Interest to Project</t>
+  </si>
+  <si>
+    <t>6. Review Project Interest</t>
+  </si>
+  <si>
+    <t>8. Post Experience</t>
+  </si>
+  <si>
+    <t>9. Post General Feedback</t>
+  </si>
+  <si>
+    <t>10. Review Project Feedback</t>
+  </si>
+  <si>
+    <t>7. Request for Certificate</t>
+  </si>
+  <si>
+    <t>13. Propose Project</t>
+  </si>
+  <si>
+    <t>15. Review Project Proposal</t>
+  </si>
+  <si>
+    <t>11. Manage Project</t>
+  </si>
+  <si>
+    <t>16. Generate Certificate</t>
+  </si>
+  <si>
+    <t>14. Search Project Proposal</t>
+  </si>
+  <si>
+    <t>17 Send  Invitation to Volunteer</t>
+  </si>
+  <si>
+    <t>UCMS</t>
+  </si>
+  <si>
+    <t>1.0.1, 1.0.2, 1.0.3, 1.0.4</t>
+  </si>
+  <si>
+    <t>1.0.5, 1.0.6, 1.0.7, 1.0.8, 1.0.9</t>
+  </si>
+  <si>
+    <t>1.0.12</t>
+  </si>
+  <si>
+    <t>1.0.14, 1.0.15, 1.0.16</t>
+  </si>
+  <si>
+    <t>1.0.17</t>
+  </si>
+  <si>
+    <t>1.0.18, 1.0.19</t>
+  </si>
+  <si>
+    <t>1.0.20, 1.0.21</t>
+  </si>
+  <si>
+    <t>1.0.22, 1.0.23, 1.0.24</t>
+  </si>
+  <si>
+    <t>1.0.25, 1.0.26, 1.0.27, 1.0.28</t>
+  </si>
+  <si>
+    <t>1.0.29</t>
+  </si>
+  <si>
+    <t>1.0.31, 1.0.32, 1.0.33</t>
+  </si>
+  <si>
+    <t>1.0.10, 1.0.11, 1.0.35</t>
+  </si>
+  <si>
+    <t>1.0.36</t>
+  </si>
+  <si>
+    <t>1.0.37, 1.0.38, 1.0.39</t>
+  </si>
+  <si>
+    <t>1.0.40, 1.0.41</t>
+  </si>
+  <si>
+    <t>1.0.42, 1.0.43, 1.0.44, 1.0.45</t>
+  </si>
+  <si>
+    <t>1.0.49 ,1.0.50 ,1.0.51 ,1.0.52 ,1.0.53 ,1.0.54 ,1.0.55 ,1.0.56</t>
+  </si>
+  <si>
+    <t>1.0.13, 1.0.40, 1.0.41</t>
+  </si>
+  <si>
+    <t>1.0.30</t>
   </si>
 </sst>
 </file>
@@ -547,6 +661,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -874,25 +993,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="29.625" customWidth="1"/>
+    <col min="5" max="5" width="29.375" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -900,637 +1019,717 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G13" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="G14" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="3"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="3"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="G21" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="G22" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="G24" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="G25" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="G26" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="E28" s="5"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="3"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="3"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="3"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="G33" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="3"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="3"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" s="5"/>
-      <c r="E38" s="3"/>
+      <c r="E38" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>37</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="E39" s="5"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="E40" s="5"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>39</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G41"/>
+  <autoFilter ref="A1:F41"/>
   <mergeCells count="3">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -1550,9 +1749,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>